<commit_message>
1.update excel once config ST
</commit_message>
<xml_diff>
--- a/ConfigFile/M5/test.xlsx
+++ b/ConfigFile/M5/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>编号</t>
   </si>
@@ -36,27 +36,6 @@
   </si>
   <si>
     <t>M5_ST锁定的AP mac地址</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>右线</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>192.168.155.3</t>
-  </si>
-  <si>
-    <t>5820</t>
-  </si>
-  <si>
-    <t>aasdasdf</t>
-  </si>
-  <si>
-    <t>192.168.155.4</t>
   </si>
 </sst>
 </file>
@@ -101,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -133,32 +112,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>